<commit_message>
Corrections Latex & ajustement budget
</commit_message>
<xml_diff>
--- a/Planification/Budget.xlsx
+++ b/Planification/Budget.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8020"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
   <si>
     <t>TOTAL</t>
   </si>
@@ -80,6 +80,9 @@
   </si>
   <si>
     <t>non-nécessaire</t>
+  </si>
+  <si>
+    <t>Électroaimant+shipping</t>
   </si>
 </sst>
 </file>
@@ -114,7 +117,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -202,11 +205,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -233,6 +249,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -540,22 +557,22 @@
   <dimension ref="C2:M29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.44140625" customWidth="1"/>
-    <col min="5" max="5" width="11.88671875" customWidth="1"/>
-    <col min="6" max="6" width="10.6640625" customWidth="1"/>
-    <col min="7" max="7" width="12.33203125" customWidth="1"/>
-    <col min="8" max="8" width="19.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.453125" customWidth="1"/>
+    <col min="5" max="5" width="11.90625" customWidth="1"/>
+    <col min="6" max="6" width="10.6328125" customWidth="1"/>
+    <col min="7" max="7" width="12.36328125" customWidth="1"/>
+    <col min="8" max="8" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="3:13" x14ac:dyDescent="0.35">
       <c r="C2" s="15" t="s">
         <v>7</v>
       </c>
@@ -567,7 +584,7 @@
       <c r="I2" s="15"/>
       <c r="J2" s="15"/>
     </row>
-    <row r="3" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="3:13" x14ac:dyDescent="0.35">
       <c r="C3" s="6" t="s">
         <v>1</v>
       </c>
@@ -593,7 +610,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:13" x14ac:dyDescent="0.35">
       <c r="C4" s="1" t="s">
         <v>11</v>
       </c>
@@ -621,7 +638,7 @@
         <v>20.550361615805258</v>
       </c>
     </row>
-    <row r="5" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:13" x14ac:dyDescent="0.35">
       <c r="C5" s="2" t="s">
         <v>12</v>
       </c>
@@ -646,7 +663,7 @@
       <c r="I5" s="13"/>
       <c r="J5" s="8"/>
     </row>
-    <row r="6" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:13" x14ac:dyDescent="0.35">
       <c r="C6" s="2" t="s">
         <v>16</v>
       </c>
@@ -680,7 +697,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:13" x14ac:dyDescent="0.35">
       <c r="C7" s="2" t="s">
         <v>18</v>
       </c>
@@ -704,15 +721,15 @@
       <c r="I7" s="13"/>
       <c r="J7" s="8"/>
       <c r="L7" s="11">
-        <f>H4+H5</f>
-        <v>9.1540435450948774</v>
+        <f>H4+H5+H10</f>
+        <v>11.906900687952021</v>
       </c>
       <c r="M7" s="11">
         <f>H6+H7</f>
         <v>29.554762744752164</v>
       </c>
     </row>
-    <row r="8" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:13" x14ac:dyDescent="0.35">
       <c r="C8" s="2" t="s">
         <v>19</v>
       </c>
@@ -741,7 +758,7 @@
         <v>44.99</v>
       </c>
     </row>
-    <row r="9" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:13" x14ac:dyDescent="0.35">
       <c r="C9" s="2" t="s">
         <v>20</v>
       </c>
@@ -770,23 +787,34 @@
         <v>20.53</v>
       </c>
     </row>
-    <row r="10" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="8"/>
+    <row r="10" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="2">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <f>12.79+6.48</f>
+        <v>19.27</v>
+      </c>
       <c r="F10" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G10" s="13"/>
+        <v>19.27</v>
+      </c>
+      <c r="G10" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="H10" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2.7528571428571427</v>
       </c>
       <c r="I10" s="13"/>
-      <c r="J10" s="8"/>
-    </row>
-    <row r="11" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="J10" s="8">
+        <v>12.79</v>
+      </c>
+    </row>
+    <row r="11" spans="3:13" x14ac:dyDescent="0.35">
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="8"/>
@@ -800,9 +828,9 @@
         <v>0</v>
       </c>
       <c r="I11" s="13"/>
-      <c r="J11" s="8"/>
-    </row>
-    <row r="12" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="J11" s="16"/>
+    </row>
+    <row r="12" spans="3:13" x14ac:dyDescent="0.35">
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="8"/>
@@ -818,7 +846,7 @@
       <c r="I12" s="13"/>
       <c r="J12" s="8"/>
     </row>
-    <row r="13" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:13" x14ac:dyDescent="0.35">
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="8"/>
@@ -834,7 +862,7 @@
       <c r="I13" s="13"/>
       <c r="J13" s="8"/>
     </row>
-    <row r="14" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:13" x14ac:dyDescent="0.35">
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="8"/>
@@ -850,7 +878,7 @@
       <c r="I14" s="13"/>
       <c r="J14" s="8"/>
     </row>
-    <row r="15" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="3:13" x14ac:dyDescent="0.35">
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="8"/>
@@ -866,7 +894,7 @@
       <c r="I15" s="13"/>
       <c r="J15" s="8"/>
     </row>
-    <row r="16" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:13" x14ac:dyDescent="0.35">
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="8"/>
@@ -882,7 +910,7 @@
       <c r="I16" s="13"/>
       <c r="J16" s="8"/>
     </row>
-    <row r="17" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="8"/>
@@ -898,7 +926,7 @@
       <c r="I17" s="13"/>
       <c r="J17" s="8"/>
     </row>
-    <row r="18" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="8"/>
@@ -914,7 +942,7 @@
       <c r="I18" s="13"/>
       <c r="J18" s="8"/>
     </row>
-    <row r="19" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="8"/>
@@ -930,7 +958,7 @@
       <c r="I19" s="13"/>
       <c r="J19" s="8"/>
     </row>
-    <row r="20" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="8"/>
@@ -946,7 +974,7 @@
       <c r="I20" s="13"/>
       <c r="J20" s="8"/>
     </row>
-    <row r="21" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="8"/>
@@ -962,7 +990,7 @@
       <c r="I21" s="13"/>
       <c r="J21" s="8"/>
     </row>
-    <row r="22" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="8"/>
@@ -978,7 +1006,7 @@
       <c r="I22" s="13"/>
       <c r="J22" s="8"/>
     </row>
-    <row r="23" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="8"/>
@@ -994,7 +1022,7 @@
       <c r="I23" s="13"/>
       <c r="J23" s="8"/>
     </row>
-    <row r="24" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="8"/>
@@ -1010,7 +1038,7 @@
       <c r="I24" s="13"/>
       <c r="J24" s="8"/>
     </row>
-    <row r="25" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="8"/>
@@ -1026,7 +1054,7 @@
       <c r="I25" s="13"/>
       <c r="J25" s="8"/>
     </row>
-    <row r="26" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="8"/>
@@ -1042,7 +1070,7 @@
       <c r="I26" s="13"/>
       <c r="J26" s="8"/>
     </row>
-    <row r="27" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
       <c r="E27" s="9"/>
@@ -1058,7 +1086,7 @@
       <c r="I27" s="14"/>
       <c r="J27" s="9"/>
     </row>
-    <row r="28" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C28" s="10"/>
       <c r="D28" s="10"/>
       <c r="E28" s="4" t="s">
@@ -1066,30 +1094,30 @@
       </c>
       <c r="F28" s="11">
         <f>SUM(F4:F27)</f>
-        <v>336.48164402892928</v>
+        <v>355.75164402892926</v>
       </c>
       <c r="G28" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H28" s="11">
         <f>SUM(H4:H27)</f>
-        <v>48.068806289847039</v>
+        <v>50.821663432704185</v>
       </c>
       <c r="I28" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J28" s="11">
         <f>SUM(J4:J27)</f>
-        <v>162.33307696830718</v>
-      </c>
-    </row>
-    <row r="29" spans="3:10" x14ac:dyDescent="0.3">
+        <v>175.12307696830717</v>
+      </c>
+    </row>
+    <row r="29" spans="3:10" x14ac:dyDescent="0.35">
       <c r="I29" s="4" t="s">
         <v>10</v>
       </c>
       <c r="J29" s="11">
         <f>300-J28</f>
-        <v>137.66692303169282</v>
+        <v>124.87692303169283</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ajout frais d'importation dans budget
</commit_message>
<xml_diff>
--- a/Planification/Budget.xlsx
+++ b/Planification/Budget.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8020"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
   <si>
     <t>TOTAL</t>
   </si>
@@ -83,6 +83,9 @@
   </si>
   <si>
     <t>Électroaimant+shipping</t>
+  </si>
+  <si>
+    <t>Importation batterie</t>
   </si>
 </sst>
 </file>
@@ -246,10 +249,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -557,34 +560,34 @@
   <dimension ref="C2:M29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="20.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.453125" customWidth="1"/>
-    <col min="5" max="5" width="11.90625" customWidth="1"/>
-    <col min="6" max="6" width="10.6328125" customWidth="1"/>
-    <col min="7" max="7" width="12.36328125" customWidth="1"/>
-    <col min="8" max="8" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.453125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.44140625" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" customWidth="1"/>
+    <col min="8" max="8" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:13" x14ac:dyDescent="0.35">
-      <c r="C2" s="15" t="s">
+    <row r="2" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C2" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-    </row>
-    <row r="3" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+    </row>
+    <row r="3" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C3" s="6" t="s">
         <v>1</v>
       </c>
@@ -610,7 +613,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="3:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C4" s="1" t="s">
         <v>11</v>
       </c>
@@ -638,7 +641,7 @@
         <v>20.550361615805258</v>
       </c>
     </row>
-    <row r="5" spans="3:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C5" s="2" t="s">
         <v>12</v>
       </c>
@@ -663,7 +666,7 @@
       <c r="I5" s="13"/>
       <c r="J5" s="8"/>
     </row>
-    <row r="6" spans="3:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C6" s="2" t="s">
         <v>16</v>
       </c>
@@ -697,7 +700,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="3:13" x14ac:dyDescent="0.35">
+    <row r="7" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C7" s="2" t="s">
         <v>18</v>
       </c>
@@ -725,11 +728,11 @@
         <v>11.906900687952021</v>
       </c>
       <c r="M7" s="11">
-        <f>H6+H7</f>
-        <v>29.554762744752164</v>
-      </c>
-    </row>
-    <row r="8" spans="3:13" x14ac:dyDescent="0.35">
+        <f>H6+H7+H11</f>
+        <v>34.526191316180736</v>
+      </c>
+    </row>
+    <row r="8" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C8" s="2" t="s">
         <v>19</v>
       </c>
@@ -758,7 +761,7 @@
         <v>44.99</v>
       </c>
     </row>
-    <row r="9" spans="3:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C9" s="2" t="s">
         <v>20</v>
       </c>
@@ -787,7 +790,7 @@
         <v>20.53</v>
       </c>
     </row>
-    <row r="10" spans="3:13" x14ac:dyDescent="0.35">
+    <row r="10" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C10" s="2" t="s">
         <v>22</v>
       </c>
@@ -814,23 +817,31 @@
         <v>12.79</v>
       </c>
     </row>
-    <row r="11" spans="3:13" x14ac:dyDescent="0.35">
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="8"/>
+    <row r="11" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="2">
+        <v>1</v>
+      </c>
+      <c r="E11" s="8">
+        <v>34.799999999999997</v>
+      </c>
       <c r="F11" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G11" s="13"/>
+        <v>34.799999999999997</v>
+      </c>
+      <c r="G11" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="H11" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4.9714285714285706</v>
       </c>
       <c r="I11" s="13"/>
-      <c r="J11" s="16"/>
-    </row>
-    <row r="12" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="J11" s="15"/>
+    </row>
+    <row r="12" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="8"/>
@@ -846,7 +857,7 @@
       <c r="I12" s="13"/>
       <c r="J12" s="8"/>
     </row>
-    <row r="13" spans="3:13" x14ac:dyDescent="0.35">
+    <row r="13" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="8"/>
@@ -862,7 +873,7 @@
       <c r="I13" s="13"/>
       <c r="J13" s="8"/>
     </row>
-    <row r="14" spans="3:13" x14ac:dyDescent="0.35">
+    <row r="14" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="8"/>
@@ -878,7 +889,7 @@
       <c r="I14" s="13"/>
       <c r="J14" s="8"/>
     </row>
-    <row r="15" spans="3:13" x14ac:dyDescent="0.35">
+    <row r="15" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="8"/>
@@ -894,7 +905,7 @@
       <c r="I15" s="13"/>
       <c r="J15" s="8"/>
     </row>
-    <row r="16" spans="3:13" x14ac:dyDescent="0.35">
+    <row r="16" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="8"/>
@@ -910,7 +921,7 @@
       <c r="I16" s="13"/>
       <c r="J16" s="8"/>
     </row>
-    <row r="17" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="8"/>
@@ -926,7 +937,7 @@
       <c r="I17" s="13"/>
       <c r="J17" s="8"/>
     </row>
-    <row r="18" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="8"/>
@@ -942,7 +953,7 @@
       <c r="I18" s="13"/>
       <c r="J18" s="8"/>
     </row>
-    <row r="19" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="8"/>
@@ -958,7 +969,7 @@
       <c r="I19" s="13"/>
       <c r="J19" s="8"/>
     </row>
-    <row r="20" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="8"/>
@@ -974,7 +985,7 @@
       <c r="I20" s="13"/>
       <c r="J20" s="8"/>
     </row>
-    <row r="21" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="21" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="8"/>
@@ -990,7 +1001,7 @@
       <c r="I21" s="13"/>
       <c r="J21" s="8"/>
     </row>
-    <row r="22" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="22" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="8"/>
@@ -1006,7 +1017,7 @@
       <c r="I22" s="13"/>
       <c r="J22" s="8"/>
     </row>
-    <row r="23" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="23" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="8"/>
@@ -1022,7 +1033,7 @@
       <c r="I23" s="13"/>
       <c r="J23" s="8"/>
     </row>
-    <row r="24" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="24" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="8"/>
@@ -1038,7 +1049,7 @@
       <c r="I24" s="13"/>
       <c r="J24" s="8"/>
     </row>
-    <row r="25" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="25" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="8"/>
@@ -1054,7 +1065,7 @@
       <c r="I25" s="13"/>
       <c r="J25" s="8"/>
     </row>
-    <row r="26" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="26" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="8"/>
@@ -1070,7 +1081,7 @@
       <c r="I26" s="13"/>
       <c r="J26" s="8"/>
     </row>
-    <row r="27" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="27" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
       <c r="E27" s="9"/>
@@ -1086,7 +1097,7 @@
       <c r="I27" s="14"/>
       <c r="J27" s="9"/>
     </row>
-    <row r="28" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="28" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C28" s="10"/>
       <c r="D28" s="10"/>
       <c r="E28" s="4" t="s">
@@ -1094,14 +1105,14 @@
       </c>
       <c r="F28" s="11">
         <f>SUM(F4:F27)</f>
-        <v>355.75164402892926</v>
+        <v>390.55164402892927</v>
       </c>
       <c r="G28" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H28" s="11">
         <f>SUM(H4:H27)</f>
-        <v>50.821663432704185</v>
+        <v>55.793092004132752</v>
       </c>
       <c r="I28" s="4" t="s">
         <v>0</v>
@@ -1111,7 +1122,7 @@
         <v>175.12307696830717</v>
       </c>
     </row>
-    <row r="29" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="29" spans="3:10" x14ac:dyDescent="0.3">
       <c r="I29" s="4" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
Création des fichiers .tex pour le remise 2 et ajustement des dossiers
</commit_message>
<xml_diff>
--- a/Planification/Budget.xlsx
+++ b/Planification/Budget.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="31">
   <si>
     <t>TOTAL</t>
   </si>
@@ -104,6 +104,9 @@
   </si>
   <si>
     <t>Connecteur batterie</t>
+  </si>
+  <si>
+    <t>Condensateurs</t>
   </si>
 </sst>
 </file>
@@ -578,7 +581,7 @@
   <dimension ref="C2:N29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -745,8 +748,8 @@
       <c r="I7" s="13"/>
       <c r="J7" s="8"/>
       <c r="L7" s="11">
-        <f>H4+H5+H10+H13+H14</f>
-        <v>21.785472116523451</v>
+        <f>H4+H5+H10+H13+H14+H16</f>
+        <v>23.071186402237736</v>
       </c>
       <c r="M7" s="11">
         <f>H6+H7+H11+F15</f>
@@ -974,20 +977,31 @@
       </c>
     </row>
     <row r="16" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="8"/>
+      <c r="C16" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="2">
+        <v>1</v>
+      </c>
+      <c r="E16" s="8">
+        <v>9</v>
+      </c>
       <c r="F16" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G16" s="13"/>
+        <v>9</v>
+      </c>
+      <c r="G16" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="H16" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.2857142857142858</v>
       </c>
       <c r="I16" s="13"/>
-      <c r="J16" s="8"/>
+      <c r="J16" s="8">
+        <f>F16</f>
+        <v>9</v>
+      </c>
     </row>
     <row r="17" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C17" s="2"/>
@@ -1173,21 +1187,21 @@
       </c>
       <c r="F28" s="11">
         <f>SUM(F4:F27)</f>
-        <v>467.20164402892931</v>
+        <v>476.20164402892931</v>
       </c>
       <c r="G28" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H28" s="11">
         <f>SUM(H4:H27)</f>
-        <v>66.743092004132748</v>
+        <v>68.02880628984704</v>
       </c>
       <c r="I28" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J28" s="11">
         <f>SUM(J4:J27)</f>
-        <v>199.77307696830718</v>
+        <v>208.77307696830718</v>
       </c>
     </row>
     <row r="29" spans="3:10" x14ac:dyDescent="0.3">
@@ -1196,7 +1210,7 @@
       </c>
       <c r="J29" s="11">
         <f>300-J28</f>
-        <v>100.22692303169282</v>
+        <v>91.22692303169282</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Corrections registre risques et budget
</commit_message>
<xml_diff>
--- a/Planification/Budget.xlsx
+++ b/Planification/Budget.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="54">
   <si>
     <t>TOTAL</t>
   </si>
@@ -97,18 +97,12 @@
     <t>PCB Manchester+pièces</t>
   </si>
   <si>
-    <t>Connecteur batterie</t>
-  </si>
-  <si>
     <t>Condensateurs</t>
   </si>
   <si>
     <t>EB-MS</t>
   </si>
   <si>
-    <t>Pièces connections</t>
-  </si>
-  <si>
     <t>PCB connections</t>
   </si>
   <si>
@@ -142,19 +136,46 @@
     <t>Vis + Boulons</t>
   </si>
   <si>
-    <t>Buck chinois</t>
-  </si>
-  <si>
     <t>Module Xbee</t>
   </si>
   <si>
-    <t>http://www.ebay.ca/itm/Xbee-S1-XB24-AUI-001-wireless-chip-with-free-u-fl-to-RP-SMA-connector-/322034412004?hash=item4afabf29e4:g:BrYAAOSwstxVVVFt</t>
-  </si>
-  <si>
     <t>Breakout board Xbee</t>
   </si>
   <si>
     <t>À vérifier sur robot</t>
+  </si>
+  <si>
+    <t>http://www.robotshop.com/ca/en/1mw-xbee-transceiver-module-trace-antenna.html</t>
+  </si>
+  <si>
+    <t>http://www.robotshop.com/ca/en/sfe-breakout-board-xbee-module.html</t>
+  </si>
+  <si>
+    <t>http://www.ebay.ca/itm/DC-DC-Adjustable-Step-up-boost-Power-Converter-Module-XL6009-Replace-LM2577-/371054648639?hash=item5664949d3f:g:nx0AAOSwGvhUJ3NQ</t>
+  </si>
+  <si>
+    <t>http://www.robotshop.com/ca/en/lynxmotion-aluminum-servo-bracket-asb-24-pair.html</t>
+  </si>
+  <si>
+    <t>http://www.robotshop.com/ca/en/aluminum-long-c-servo-bracket-asb-05.html</t>
+  </si>
+  <si>
+    <t>Brackets servomoteur2(1/2 sur le robot</t>
+  </si>
+  <si>
+    <t>Brackets servomoteur(1/2 sur le robot)</t>
+  </si>
+  <si>
+    <t>Connecteur batterie (chargeur)</t>
+  </si>
+  <si>
+    <t>Buck pour xbee</t>
+  </si>
+  <si>
+    <t>Avec frais d'importations ? Sans = 30.84</t>
+  </si>
+  <si>
+    <t>Pièces connections(pas sur robot)</t>
   </si>
 </sst>
 </file>
@@ -348,10 +369,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -659,15 +680,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:N35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="O20" sqref="O20"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="4.33203125" customWidth="1"/>
     <col min="2" max="2" width="4.6640625" customWidth="1"/>
-    <col min="3" max="3" width="27" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.44140625" customWidth="1"/>
     <col min="5" max="5" width="11.88671875" customWidth="1"/>
     <col min="6" max="6" width="10.6640625" customWidth="1"/>
@@ -678,16 +699,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
     </row>
     <row r="3" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C3" s="6" t="s">
@@ -739,8 +760,11 @@
       </c>
       <c r="I4" s="12"/>
       <c r="J4" s="7">
-        <f>2*E4</f>
-        <v>20.550361615805258</v>
+        <f>F4</f>
+        <v>30.825542423707887</v>
+      </c>
+      <c r="K4" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="3:14" x14ac:dyDescent="0.3">
@@ -780,7 +804,7 @@
         <v>169.03333921326515</v>
       </c>
       <c r="F6" s="8">
-        <f t="shared" ref="F6:F31" si="0">D6*E6</f>
+        <f t="shared" ref="F6:F33" si="0">D6*E6</f>
         <v>169.03333921326515</v>
       </c>
       <c r="G6" s="13" t="s">
@@ -802,7 +826,7 @@
         <v>15</v>
       </c>
       <c r="N6" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="3:14" x14ac:dyDescent="0.3">
@@ -965,7 +989,7 @@
         <v>9</v>
       </c>
       <c r="G12" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H12" s="8">
         <f t="shared" si="1"/>
@@ -999,7 +1023,7 @@
       </c>
       <c r="I13" s="13"/>
       <c r="J13" s="8">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="3:14" x14ac:dyDescent="0.3">
@@ -1029,7 +1053,7 @@
     </row>
     <row r="15" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C15" s="2" t="s">
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="D15" s="2">
         <v>1</v>
@@ -1049,14 +1073,11 @@
         <v>0.21428571428571427</v>
       </c>
       <c r="I15" s="13"/>
-      <c r="J15" s="8">
-        <f>F15</f>
-        <v>1.5</v>
-      </c>
+      <c r="J15" s="8"/>
     </row>
     <row r="16" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C16" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D16" s="2">
         <v>1</v>
@@ -1077,16 +1098,15 @@
       </c>
       <c r="I16" s="13"/>
       <c r="J16" s="8">
-        <f>F16</f>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="K16" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C17" s="2" t="s">
-        <v>30</v>
+        <v>53</v>
       </c>
       <c r="D17" s="2">
         <v>1</v>
@@ -1106,14 +1126,11 @@
         <v>0.5714285714285714</v>
       </c>
       <c r="I17" s="13"/>
-      <c r="J17" s="8">
-        <f>E17</f>
-        <v>4</v>
-      </c>
+      <c r="J17" s="8"/>
     </row>
     <row r="18" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C18" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D18" s="2">
         <v>1</v>
@@ -1137,7 +1154,7 @@
     </row>
     <row r="19" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C19" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D19" s="2">
         <v>1</v>
@@ -1161,7 +1178,7 @@
     </row>
     <row r="20" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C20" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D20" s="2">
         <v>1</v>
@@ -1185,7 +1202,7 @@
     </row>
     <row r="21" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C21" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D21" s="2">
         <v>1</v>
@@ -1209,7 +1226,7 @@
     </row>
     <row r="22" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C22" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D22" s="2">
         <v>1</v>
@@ -1233,7 +1250,7 @@
     </row>
     <row r="23" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C23" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D23" s="2">
         <v>1</v>
@@ -1260,7 +1277,7 @@
     </row>
     <row r="24" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C24" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D24" s="2">
         <v>1</v>
@@ -1284,7 +1301,7 @@
     </row>
     <row r="25" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C25" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D25" s="2">
         <v>1</v>
@@ -1297,7 +1314,7 @@
         <v>20</v>
       </c>
       <c r="G25" s="13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H25" s="8">
         <f t="shared" si="1"/>
@@ -1308,7 +1325,7 @@
     </row>
     <row r="26" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C26" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D26" s="2">
         <v>1</v>
@@ -1332,7 +1349,7 @@
     </row>
     <row r="27" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C27" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D27" s="3">
         <v>1</v>
@@ -1352,42 +1369,41 @@
         <v>0.68285714285714294</v>
       </c>
       <c r="I27" s="14"/>
-      <c r="J27" s="9">
-        <f>F27</f>
-        <v>4.78</v>
-      </c>
+      <c r="J27" s="9"/>
     </row>
     <row r="28" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C28" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D28" s="3">
         <v>2</v>
       </c>
       <c r="E28" s="9">
-        <v>15.82</v>
+        <v>33.270000000000003</v>
       </c>
       <c r="F28" s="9">
         <f t="shared" si="0"/>
-        <v>31.64</v>
+        <v>66.540000000000006</v>
       </c>
       <c r="G28" s="14"/>
       <c r="H28" s="9">
         <f t="shared" si="1"/>
-        <v>4.5200000000000005</v>
-      </c>
-      <c r="I28" s="14"/>
+        <v>9.5057142857142871</v>
+      </c>
+      <c r="I28" s="14" t="s">
+        <v>21</v>
+      </c>
       <c r="J28" s="9">
         <f>F28</f>
-        <v>31.64</v>
-      </c>
-      <c r="K28" s="20" t="s">
-        <v>44</v>
+        <v>66.540000000000006</v>
+      </c>
+      <c r="K28" s="19" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="29" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C29" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D29" s="2">
         <v>1</v>
@@ -1407,11 +1423,13 @@
         <v>3.4285714285714284</v>
       </c>
       <c r="I29" s="13"/>
-      <c r="J29" s="8"/>
+      <c r="J29" s="8">
+        <v>4</v>
+      </c>
     </row>
     <row r="30" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C30" s="2" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="D30" s="2">
         <v>1</v>
@@ -1428,15 +1446,19 @@
         <f>F30/7</f>
         <v>0.2857142857142857</v>
       </c>
-      <c r="I30" s="13"/>
+      <c r="I30" s="13" t="s">
+        <v>21</v>
+      </c>
       <c r="J30" s="8">
-        <f>E30</f>
-        <v>2</v>
+        <v>1.77</v>
+      </c>
+      <c r="K30" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="31" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C31" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D31" s="2">
         <v>2</v>
@@ -1453,74 +1475,120 @@
         <f>F31/7</f>
         <v>1.122857142857143</v>
       </c>
-      <c r="I31" s="13"/>
+      <c r="I31" s="13" t="s">
+        <v>21</v>
+      </c>
       <c r="J31" s="8">
         <f>F31</f>
         <v>7.86</v>
       </c>
+      <c r="K31" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="32" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="8"/>
-      <c r="F32" s="8"/>
-      <c r="G32" s="13"/>
-      <c r="H32" s="8"/>
-      <c r="I32" s="13"/>
-      <c r="J32" s="8"/>
-    </row>
-    <row r="33" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C33" s="16"/>
-      <c r="D33" s="16"/>
-      <c r="E33" s="17"/>
-      <c r="F33" s="17"/>
-      <c r="G33" s="18"/>
-      <c r="H33" s="17"/>
-      <c r="I33" s="18"/>
-      <c r="J33" s="17"/>
-    </row>
-    <row r="34" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C32" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D32" s="2">
+        <v>1</v>
+      </c>
+      <c r="E32" s="8">
+        <v>5.76</v>
+      </c>
+      <c r="F32" s="8">
+        <f t="shared" si="0"/>
+        <v>5.76</v>
+      </c>
+      <c r="G32" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="H32" s="8">
+        <f>F32/7</f>
+        <v>0.82285714285714284</v>
+      </c>
+      <c r="I32" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="J32" s="8">
+        <f>F32/2</f>
+        <v>2.88</v>
+      </c>
+      <c r="K32" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="33" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C33" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="D33" s="16">
+        <v>1</v>
+      </c>
+      <c r="E33" s="17">
+        <v>5.3</v>
+      </c>
+      <c r="F33" s="17">
+        <f t="shared" si="0"/>
+        <v>5.3</v>
+      </c>
+      <c r="G33" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="H33" s="17">
+        <f>F33/7</f>
+        <v>0.75714285714285712</v>
+      </c>
+      <c r="I33" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="J33" s="17">
+        <f>F33/2</f>
+        <v>2.65</v>
+      </c>
+      <c r="K33" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="34" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C34" s="10"/>
       <c r="D34" s="10"/>
       <c r="E34" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F34" s="11">
-        <f>SUM(F4:F31)</f>
-        <v>656.68164402892933</v>
+        <f>SUM(F4:F33)</f>
+        <v>702.64164402892925</v>
       </c>
       <c r="G34" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H34" s="11">
-        <f>SUM(H4:H31)</f>
-        <v>93.811663432704208</v>
+        <f>SUM(H4:H33)</f>
+        <v>100.3773777184185</v>
       </c>
       <c r="I34" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J34" s="11">
         <f>SUM(J4:J33)</f>
-        <v>255.10307696830716</v>
-      </c>
-    </row>
-    <row r="35" spans="3:10" x14ac:dyDescent="0.3">
+        <v>297.29825777620977</v>
+      </c>
+    </row>
+    <row r="35" spans="3:11" x14ac:dyDescent="0.3">
       <c r="I35" s="4" t="s">
         <v>10</v>
       </c>
       <c r="J35" s="11">
         <f>300-J34</f>
-        <v>44.896923031692836</v>
+        <v>2.7017422237902338</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="C2:J2"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="K28" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ajouts textes et photos
</commit_message>
<xml_diff>
--- a/Planification/Budget.xlsx
+++ b/Planification/Budget.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Portrait général" sheetId="1" r:id="rId1"/>
@@ -459,14 +459,14 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -775,8 +775,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:N35"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="J34" sqref="J34"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -794,16 +794,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
     </row>
     <row r="3" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C3" s="6" t="s">
@@ -1705,7 +1705,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
@@ -2019,7 +2019,7 @@
       <c r="C18" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="D18" s="24">
+      <c r="D18" s="23">
         <v>1</v>
       </c>
       <c r="E18" s="17">
@@ -2031,16 +2031,16 @@
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="E19" s="25" t="s">
+      <c r="E19" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="F19" s="26">
+      <c r="F19" s="25">
         <f>SUM(F3:F18)</f>
         <v>288.33169874999999</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C21" s="27" t="s">
+      <c r="C21" s="26" t="s">
         <v>50</v>
       </c>
       <c r="D21">

</xml_diff>